<commit_message>
minor fixes for sampleProjectPosts
</commit_message>
<xml_diff>
--- a/jvm/src/main/resources/sample-data-demo.xlsx
+++ b/jvm/src/main/resources/sample-data-demo.xlsx
@@ -7177,9 +7177,6 @@
     <t>skillsId</t>
   </si>
   <si>
-    <t xml:space="preserve"> true</t>
-  </si>
-  <si>
     <t>referralId</t>
   </si>
   <si>
@@ -7214,6 +7211,9 @@
   </si>
   <si>
     <t>&lt;above&gt;</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -7619,6 +7619,14 @@
   <dxfs count="61">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -7642,14 +7650,6 @@
       <font>
         <b val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -9007,8 +9007,8 @@
     <tableColumn id="15" name="referralId" dataDxfId="7"/>
     <tableColumn id="16" name="contractType" dataDxfId="6"/>
     <tableColumn id="17" name="budget" dataDxfId="5"/>
-    <tableColumn id="18" name="json" dataDxfId="4">
-      <calculatedColumnFormula>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": "" "&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skillsId]]&amp;""": """&amp;Table5[[#This Row],[skillsId]]&amp;""", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referralId]]&amp;""": """&amp;Table5[[#This Row],[referralId]]&amp;""", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</calculatedColumnFormula>
+    <tableColumn id="18" name="json" dataDxfId="0">
+      <calculatedColumnFormula>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": """&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skillsId]]&amp;""": """&amp;Table5[[#This Row],[skillsId]]&amp;""", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referralId]]&amp;""": """&amp;Table5[[#This Row],[referralId]]&amp;""", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9019,12 +9019,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:F357" totalsRowShown="0">
   <autoFilter ref="A1:F357"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="3"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
     <tableColumn id="3" name="L1"/>
-    <tableColumn id="4" name="Type" dataDxfId="2"/>
-    <tableColumn id="5" name="Value" dataDxfId="1"/>
+    <tableColumn id="4" name="Type" dataDxfId="3"/>
+    <tableColumn id="5" name="Value" dataDxfId="2"/>
     <tableColumn id="6" name="Comment"/>
-    <tableColumn id="2" name="Data" dataDxfId="0">
+    <tableColumn id="2" name="Data" dataDxfId="1">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Type]]="functor","{""id"" : """&amp;Table6[[#This Row],[ID]]&amp;""", ""functor"" : """ &amp;Table6[[#This Row],[L1]]&amp;""",  ""components"" : [",IF(Table6[[#This Row],[Type]]="]},","]}, ",IF(Table6[[#This Row],[Type]]="]}","]}",IF(MATCH(Table6[[#This Row],[Type]],{"integer","float","string","date","boolean"},0),"{""id"" : """&amp;Table6[[#This Row],[ID]]&amp;""" , ""functor"" : """&amp;Table6[[#This Row],[L1]]&amp;""" , ""components"": [ { ""value"": """ &amp; Table6[[#This Row],[Value]]&amp;""", ""type"" : """&amp;Table6[[#This Row],[Type]]&amp;""" } ] } "&amp;IF(OR($C3="]}",$C3="]},"),""," , ")))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -22458,8 +22458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22528,16 +22528,16 @@
         <v>2235</v>
       </c>
       <c r="O1" t="s">
+        <v>2363</v>
+      </c>
+      <c r="P1" t="s">
         <v>2364</v>
-      </c>
-      <c r="P1" t="s">
-        <v>2365</v>
       </c>
       <c r="Q1" t="s">
         <v>2069</v>
       </c>
       <c r="R1" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -22548,10 +22548,10 @@
         <v>2354</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="E2" s="96" t="s">
         <v>2272</v>
@@ -22569,22 +22569,22 @@
         <v>2070</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="K2" s="67" t="s">
         <v>2310</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="M2" s="67" t="s">
         <v>2271</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>2363</v>
+      <c r="N2" s="67" t="s">
+        <v>2375</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="P2" s="67" t="s">
         <v>2000</v>
@@ -22593,8 +22593,8 @@
         <v>2350.3000000000002</v>
       </c>
       <c r="R2" s="5" t="str">
-        <f>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": "" "&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skillsId]]&amp;""": """&amp;Table5[[#This Row],[skillsId]]&amp;""", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referralId]]&amp;""": """&amp;Table5[[#This Row],[referralId]]&amp;""", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</f>
-        <v>{"id": "d2b255ca-dde8-4919-9e5d-a0a62d5d7c12", "type": " PROJECT", "summary": "This is new project", "description": "Need scala developer to implement a centralized repository for a big financial institution. ", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skillsId": "[\"4416192b-9dec-49b0-9d13-fb0815af6c3f\", \"3c91c578-2d39-42d4-adb0-9071d9eb116a\", \"b48bfe5a-15fa-4d8e-b253-752b51c2b94b\"]", "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": " true", "referralId": "[\"40c96981-ca91-4083-9dfc-76826df0f432\",\"c6a3c02e-5724-4a35-adc7-ddc37d3c721b\"]", "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
+        <f>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": """&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skillsId]]&amp;""": """&amp;Table5[[#This Row],[skillsId]]&amp;""", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referralId]]&amp;""": """&amp;Table5[[#This Row],[referralId]]&amp;""", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</f>
+        <v>{"id": "d2b255ca-dde8-4919-9e5d-a0a62d5d7c12", "type": "PROJECT", "summary": "This is new project", "description": "Need scala developer to implement a centralized repository for a big financial institution. ", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skillsId": "[\"4416192b-9dec-49b0-9d13-fb0815af6c3f\", \"3c91c578-2d39-42d4-adb0-9071d9eb116a\", \"b48bfe5a-15fa-4d8e-b253-752b51c2b94b\"]", "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referralId": "[\"40c96981-ca91-4083-9dfc-76826df0f432\",\"c6a3c02e-5724-4a35-adc7-ddc37d3c721b\"]", "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -22605,10 +22605,10 @@
         <v>2354</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>2368</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>2369</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>2370</v>
       </c>
       <c r="E3" s="96" t="s">
         <v>2272</v>
@@ -22626,22 +22626,22 @@
         <v>2070</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="K3" s="67" t="s">
         <v>2310</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="M3" s="67" t="s">
         <v>2271</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>2363</v>
+      <c r="N3" s="67" t="s">
+        <v>2375</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="P3" s="67" t="s">
         <v>2000</v>
@@ -22650,18 +22650,18 @@
         <v>2350.3000000000002</v>
       </c>
       <c r="R3" s="5" t="str">
-        <f>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": "" "&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skillsId]]&amp;""": """&amp;Table5[[#This Row],[skillsId]]&amp;""", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referralId]]&amp;""": """&amp;Table5[[#This Row],[referralId]]&amp;""", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</f>
-        <v>{"id": "e231791e-2719-4503-ad8f-8dd55a53901e", "type": " PROJECT", "summary": "This is an even newer project", "description": "Need scala developer to implement a small program to replace the Federal Reserve. ", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skillsId": "[\"4416192b-9dec-49b0-9d13-fb0815af6c3f\", \"3c91c578-2d39-42d4-adb0-9071d9eb116a\", \"b48bfe5a-15fa-4d8e-b253-752b51c2b94b\"]", "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": " true", "referralId": "[\"40c96981-ca91-4083-9dfc-76826df0f432\",\"c6a3c02e-5724-4a35-adc7-ddc37d3c721b\"]", "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
+        <f>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": """&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skillsId]]&amp;""": """&amp;Table5[[#This Row],[skillsId]]&amp;""", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referralId]]&amp;""": """&amp;Table5[[#This Row],[referralId]]&amp;""", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</f>
+        <v>{"id": "e231791e-2719-4503-ad8f-8dd55a53901e", "type": "PROJECT", "summary": "This is an even newer project", "description": "Need scala developer to implement a small program to replace the Federal Reserve. ", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skillsId": "[\"4416192b-9dec-49b0-9d13-fb0815af6c3f\", \"3c91c578-2d39-42d4-adb0-9071d9eb116a\", \"b48bfe5a-15fa-4d8e-b253-752b51c2b94b\"]", "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referralId": "[\"40c96981-ca91-4083-9dfc-76826df0f432\",\"c6a3c02e-5724-4a35-adc7-ddc37d3c721b\"]", "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated job sample data
</commit_message>
<xml_diff>
--- a/jvm/src/main/resources/sample-data-demo.xlsx
+++ b/jvm/src/main/resources/sample-data-demo.xlsx
@@ -25,7 +25,7 @@
     <sheet name="to do" sheetId="8" r:id="rId11"/>
     <sheet name="export template" sheetId="4" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3990" uniqueCount="2448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3990" uniqueCount="2449">
   <si>
     <t>firstName</t>
   </si>
@@ -7152,9 +7152,6 @@
     <t>updated</t>
   </si>
   <si>
-    <t>PROJECT</t>
-  </si>
-  <si>
     <t>summary</t>
   </si>
   <si>
@@ -7423,16 +7420,22 @@
     <t>Then paste that into the mock file in the pageOfPosts property (in proper syntax).</t>
   </si>
   <si>
-    <t>Need real, real good javascript developer to implement a centralized repository for a big financial institution.</t>
-  </si>
-  <si>
-    <t>Need a scala developer to implement a decentralized repository for a trillion dollar financial use case.</t>
-  </si>
-  <si>
-    <t>This is good project</t>
-  </si>
-  <si>
-    <t>This is an even better project</t>
+    <t>Front-end web page for Blockchain network currently set up on cloud server</t>
+  </si>
+  <si>
+    <t>Developers for a Framework for developing p2p Front-Ends for Blockchain APPs</t>
+  </si>
+  <si>
+    <t>Project-Hourly</t>
+  </si>
+  <si>
+    <t>Part-Time</t>
+  </si>
+  <si>
+    <t>Develop a front-end web interface for a game to be played by employees of the organisation. All back-end data processing is done in a simplified version of Blockchain environment that is currently set up and fully operational on Microsoft Azure cloud server.  Project description: In order to play the game a user must have a fitness sportsband and have it registered under the organisation’s corporate group. ...</t>
+  </si>
+  <si>
+    <t>We invite you to join Fermat, a community building an OS extension able to run p2p mobile APPs  like Uber without Uber Inc., or  Airbnb without Airbnb Inc , or Linkedin, or Tinder, etc,  you name it, all of them without the middle-men.  Each component of the system is owned by whoever writes their code. Later, devs receive a stream of micro-payments from end-users around the globe using APPs built with their components.  Join us and learn bitcoin and blockchain technology and be part of one of the fastest growing open source projects.: https://github.com/Fermat-ORG/fermat ...</t>
   </si>
 </sst>
 </file>
@@ -10134,6 +10137,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -10169,6 +10189,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -30246,7 +30283,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30279,16 +30316,16 @@
         <v>2341</v>
       </c>
       <c r="C1" t="s">
+        <v>2354</v>
+      </c>
+      <c r="D1" t="s">
         <v>2355</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2356</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2357</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2358</v>
       </c>
       <c r="G1" t="s">
         <v>2212</v>
@@ -30297,13 +30334,13 @@
         <v>2320</v>
       </c>
       <c r="I1" t="s">
+        <v>2358</v>
+      </c>
+      <c r="J1" t="s">
         <v>2359</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>2360</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2361</v>
       </c>
       <c r="L1" t="s">
         <v>347</v>
@@ -30315,16 +30352,16 @@
         <v>2235</v>
       </c>
       <c r="O1" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="P1" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="Q1" t="s">
         <v>2069</v>
       </c>
       <c r="R1" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -30332,13 +30369,13 @@
         <v>2001</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2354</v>
+        <v>2445</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>2446</v>
+        <v>2443</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>2444</v>
+        <v>2447</v>
       </c>
       <c r="E2" s="96" t="s">
         <v>2272</v>
@@ -30356,22 +30393,22 @@
         <v>2070</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="K2" s="67" t="s">
         <v>2310</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="M2" s="67" t="s">
         <v>2271</v>
       </c>
       <c r="N2" s="67" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="P2" s="67" t="s">
         <v>2000</v>
@@ -30381,7 +30418,7 @@
       </c>
       <c r="R2" s="5" t="str">
         <f>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": """&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skills]]&amp;""": "&amp;Table5[[#This Row],[skills]]&amp;", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referents]]&amp;""": "&amp;Table5[[#This Row],[referents]]&amp;", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</f>
-        <v>{"id": "d2b255ca-dde8-4919-9e5d-a0a62d5d7c12", "type": "PROJECT", "summary": "This is good project", "description": "Need real, real good javascript developer to implement a centralized repository for a big financial institution.", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skills": [{"skillId": "4416192b-9dec-49b0-9d13-fb0815af6c3f", "skillName":"Java"}, {"skillId": "3c91c578-2d39-42d4-adb0-9071d9eb116a", "skillName":"Financial Apps"}, {"skillId": "b48bfe5a-15fa-4d8e-b253-752b51c2b94b", "skillName":"cryptography"}], "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referents": [{"referentId":"40c96981-ca91-4083-9dfc-76826df0f432", "referentName":"Britta"},{"referentId":"c6a3c02e-5724-4a35-adc7-ddc37d3c721b","referentName":"Jane Best"}], "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
+        <v>{"id": "d2b255ca-dde8-4919-9e5d-a0a62d5d7c12", "type": "Project-Hourly", "summary": "Front-end web page for Blockchain network currently set up on cloud server", "description": "Develop a front-end web interface for a game to be played by employees of the organisation. All back-end data processing is done in a simplified version of Blockchain environment that is currently set up and fully operational on Microsoft Azure cloud server.  Project description: In order to play the game a user must have a fitness sportsband and have it registered under the organisation’s corporate group. ...", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skills": [{"skillId": "4416192b-9dec-49b0-9d13-fb0815af6c3f", "skillName":"Java"}, {"skillId": "3c91c578-2d39-42d4-adb0-9071d9eb116a", "skillName":"Financial Apps"}, {"skillId": "b48bfe5a-15fa-4d8e-b253-752b51c2b94b", "skillName":"cryptography"}], "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referents": [{"referentId":"40c96981-ca91-4083-9dfc-76826df0f432", "referentName":"Britta"},{"referentId":"c6a3c02e-5724-4a35-adc7-ddc37d3c721b","referentName":"Jane Best"}], "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -30389,13 +30426,13 @@
         <v>1999</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2354</v>
+        <v>2446</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>2447</v>
+        <v>2444</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>2445</v>
+        <v>2448</v>
       </c>
       <c r="E3" s="96" t="s">
         <v>2272</v>
@@ -30413,22 +30450,22 @@
         <v>2070</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="K3" s="67" t="s">
         <v>2310</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="M3" s="67" t="s">
         <v>2271</v>
       </c>
       <c r="N3" s="67" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="P3" s="67" t="s">
         <v>2000</v>
@@ -30438,17 +30475,17 @@
       </c>
       <c r="R3" s="5" t="str">
         <f>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": """&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skills]]&amp;""": "&amp;Table5[[#This Row],[skills]]&amp;", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referents]]&amp;""": "&amp;Table5[[#This Row],[referents]]&amp;", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</f>
-        <v>{"id": "e231791e-2719-4503-ad8f-8dd55a53901e", "type": "PROJECT", "summary": "This is an even better project", "description": "Need a scala developer to implement a decentralized repository for a trillion dollar financial use case.", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skills": [{"skillId": "4416192b-9dec-49b0-9d13-fb0815af6c3f", "skillName":"Java"}, {"skillId": "3c91c578-2d39-42d4-adb0-9071d9eb116a", "skillName":"Financial Apps"}, {"skillId": "b48bfe5a-15fa-4d8e-b253-752b51c2b94b", "skillName":"cryptography"}], "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referents": [{"referentId":"40c96981-ca91-4083-9dfc-76826df0f432", "referentName":"Britta"},{"referentId":"c6a3c02e-5724-4a35-adc7-ddc37d3c721b","referentName":"Jane Best"}], "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
+        <v>{"id": "e231791e-2719-4503-ad8f-8dd55a53901e", "type": "Part-Time", "summary": "Developers for a Framework for developing p2p Front-Ends for Blockchain APPs", "description": "We invite you to join Fermat, a community building an OS extension able to run p2p mobile APPs  like Uber without Uber Inc., or  Airbnb without Airbnb Inc , or Linkedin, or Tinder, etc,  you name it, all of them without the middle-men.  Each component of the system is owned by whoever writes their code. Later, devs receive a stream of micro-payments from end-users around the globe using APPs built with their components.  Join us and learn bitcoin and blockchain technology and be part of one of the fastest growing open source projects.: https://github.com/Fermat-ORG/fermat ...", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skills": [{"skillId": "4416192b-9dec-49b0-9d13-fb0815af6c3f", "skillName":"Java"}, {"skillId": "3c91c578-2d39-42d4-adb0-9071d9eb116a", "skillName":"Financial Apps"}, {"skillId": "b48bfe5a-15fa-4d8e-b253-752b51c2b94b", "skillName":"cryptography"}], "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referents": [{"referentId":"40c96981-ca91-4083-9dfc-76826df0f432", "referentName":"Britta"},{"referentId":"c6a3c02e-5724-4a35-adc7-ddc37d3c721b","referentName":"Jane Best"}], "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -30458,32 +30495,32 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="56" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
     </row>
   </sheetData>
@@ -30513,103 +30550,103 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="K2" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="G3" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="K3" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="G5" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="G6" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="G7" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="G8" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="G11" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="G12" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="G13" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="G14" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -30619,87 +30656,87 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -30709,17 +30746,17 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
     </row>
   </sheetData>
@@ -30746,12 +30783,12 @@
   <sheetData>
     <row r="3" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="98" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="4" spans="2:16" s="105" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="103" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="C4" s="104"/>
       <c r="D4" s="104"/>
@@ -30761,12 +30798,12 @@
     </row>
     <row r="5" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="98" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="6" spans="2:16" s="105" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="103" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="C6" s="104"/>
       <c r="D6" s="104"/>
@@ -30776,12 +30813,12 @@
     </row>
     <row r="7" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="98" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="8" spans="2:16" s="105" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="103" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="C8" s="104"/>
       <c r="D8" s="104"/>
@@ -30791,16 +30828,16 @@
     </row>
     <row r="9" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="98" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="10" spans="2:16" s="105" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="103"/>
       <c r="C10" s="113" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="D10" s="115" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="E10" s="116"/>
       <c r="F10" s="116"/>
@@ -30809,146 +30846,146 @@
     </row>
     <row r="11" spans="2:16" s="105" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="106" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="C11" s="114"/>
       <c r="D11" s="109" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="E11" s="109" t="s">
+        <v>2425</v>
+      </c>
+      <c r="F11" s="109" t="s">
         <v>2426</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="G11" s="109" t="s">
         <v>2427</v>
       </c>
-      <c r="G11" s="109" t="s">
+      <c r="H11" s="109" t="s">
         <v>2428</v>
-      </c>
-      <c r="H11" s="109" t="s">
-        <v>2429</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="99" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="C12" s="111" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="D12" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="E12" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="F12" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="G12" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="H12" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="13" spans="2:16" s="105" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="107" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="C13" s="112" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="D13" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="E13" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="F13" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="G13" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="H13" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="P13" s="105" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="100" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="C14" s="111" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="D14" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="E14" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="F14" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="G14" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="H14" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="15" spans="2:16" s="105" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="107" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="C15" s="112" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="D15" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="E15" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="F15" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="G15" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="H15" s="108" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="100" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="C16" s="111" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="D16" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="E16" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="F16" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="G16" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="H16" s="102" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="17" spans="2:7" s="105" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="110" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="C17" s="104"/>
       <c r="D17" s="104"/>

</xml_diff>

<commit_message>
updated sample data for jobs
</commit_message>
<xml_diff>
--- a/jvm/src/main/resources/sample-data-demo.xlsx
+++ b/jvm/src/main/resources/sample-data-demo.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3990" uniqueCount="2449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4006" uniqueCount="2452">
   <si>
     <t>firstName</t>
   </si>
@@ -7423,19 +7423,28 @@
     <t>Front-end web page for Blockchain network currently set up on cloud server</t>
   </si>
   <si>
-    <t>Developers for a Framework for developing p2p Front-Ends for Blockchain APPs</t>
-  </si>
-  <si>
     <t>Project-Hourly</t>
   </si>
   <si>
-    <t>Part-Time</t>
-  </si>
-  <si>
     <t>Develop a front-end web interface for a game to be played by employees of the organisation. All back-end data processing is done in a simplified version of Blockchain environment that is currently set up and fully operational on Microsoft Azure cloud server.  Project description: In order to play the game a user must have a fitness sportsband and have it registered under the organisation’s corporate group. ...</t>
   </si>
   <si>
-    <t>We invite you to join Fermat, a community building an OS extension able to run p2p mobile APPs  like Uber without Uber Inc., or  Airbnb without Airbnb Inc , or Linkedin, or Tinder, etc,  you name it, all of them without the middle-men.  Each component of the system is owned by whoever writes their code. Later, devs receive a stream of micro-payments from end-users around the globe using APPs built with their components.  Join us and learn bitcoin and blockchain technology and be part of one of the fastest growing open source projects.: https://github.com/Fermat-ORG/fermat ...</t>
+    <t>Contest – online sales team/tools for bitcoin development</t>
+  </si>
+  <si>
+    <t>To join this contest just register at https://www.greatcoincontest.io, click at the product you want to sell and generate your reff link. This reff link also works with other products on the site. Once your id is in buyer’s cookies, you’ll get 10% of every sale from this person on the marketplace.  When? Contest starts 24.2. 2016 0:00 UTC and ends 24.3. 2016 23:59 UTC. Winner will be contacted right after that. ...</t>
+  </si>
+  <si>
+    <t>Contest</t>
+  </si>
+  <si>
+    <t>Help test Bitcoin as payment for my travel-related business</t>
+  </si>
+  <si>
+    <t>e231791e-2719-4503-ad8f-8dd55a53901a</t>
+  </si>
+  <si>
+    <t>This project can be a huge project but same time can easily fail, so please PM with your skills, I will provide you the project details and if you consider it’s a good idea we can start work right away</t>
   </si>
 </sst>
 </file>
@@ -7762,7 +7771,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -8007,38 +8016,13 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="61">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -8355,6 +8339,32 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -10016,27 +10026,27 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:R3" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A1:R3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:R4" totalsRowShown="0" dataDxfId="18">
+  <autoFilter ref="A1:R4"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="id" dataDxfId="21"/>
-    <tableColumn id="2" name="type" dataDxfId="20"/>
-    <tableColumn id="3" name="summary" dataDxfId="19"/>
-    <tableColumn id="4" name="description" dataDxfId="18"/>
-    <tableColumn id="5" name="postedDate" dataDxfId="17"/>
-    <tableColumn id="6" name="broadcastDate" dataDxfId="16"/>
-    <tableColumn id="7" name="startDate" dataDxfId="15"/>
-    <tableColumn id="8" name="endDate" dataDxfId="14"/>
-    <tableColumn id="9" name="currency" dataDxfId="13"/>
-    <tableColumn id="10" name="location" dataDxfId="12"/>
-    <tableColumn id="11" name="isPayoutInPieces" dataDxfId="11"/>
-    <tableColumn id="12" name="skills" dataDxfId="10"/>
-    <tableColumn id="13" name="posterId" dataDxfId="9"/>
-    <tableColumn id="14" name="canForward" dataDxfId="8"/>
-    <tableColumn id="15" name="referents" dataDxfId="7"/>
-    <tableColumn id="16" name="contractType" dataDxfId="6"/>
-    <tableColumn id="17" name="budget" dataDxfId="5"/>
-    <tableColumn id="18" name="json" dataDxfId="4">
+    <tableColumn id="1" name="id" dataDxfId="17"/>
+    <tableColumn id="2" name="type" dataDxfId="16"/>
+    <tableColumn id="3" name="summary" dataDxfId="15"/>
+    <tableColumn id="4" name="description" dataDxfId="14"/>
+    <tableColumn id="5" name="postedDate" dataDxfId="13"/>
+    <tableColumn id="6" name="broadcastDate" dataDxfId="12"/>
+    <tableColumn id="7" name="startDate" dataDxfId="11"/>
+    <tableColumn id="8" name="endDate" dataDxfId="10"/>
+    <tableColumn id="9" name="currency" dataDxfId="9"/>
+    <tableColumn id="10" name="location" dataDxfId="8"/>
+    <tableColumn id="11" name="isPayoutInPieces" dataDxfId="7"/>
+    <tableColumn id="12" name="skills" dataDxfId="6"/>
+    <tableColumn id="13" name="posterId" dataDxfId="5"/>
+    <tableColumn id="14" name="canForward" dataDxfId="4"/>
+    <tableColumn id="15" name="referents" dataDxfId="3"/>
+    <tableColumn id="16" name="contractType" dataDxfId="2"/>
+    <tableColumn id="17" name="budget" dataDxfId="1"/>
+    <tableColumn id="18" name="json" dataDxfId="0">
       <calculatedColumnFormula>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": """&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skills]]&amp;""": "&amp;Table5[[#This Row],[skills]]&amp;", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referents]]&amp;""": "&amp;Table5[[#This Row],[referents]]&amp;", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10048,12 +10058,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:F357" totalsRowShown="0">
   <autoFilter ref="A1:F357"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="3"/>
+    <tableColumn id="1" name="ID" dataDxfId="22"/>
     <tableColumn id="3" name="L1"/>
-    <tableColumn id="4" name="Type" dataDxfId="2"/>
-    <tableColumn id="5" name="Value" dataDxfId="1"/>
+    <tableColumn id="4" name="Type" dataDxfId="21"/>
+    <tableColumn id="5" name="Value" dataDxfId="20"/>
     <tableColumn id="6" name="Comment"/>
-    <tableColumn id="2" name="Data" dataDxfId="0">
+    <tableColumn id="2" name="Data" dataDxfId="19">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Type]]="functor","{""id"" : """&amp;Table6[[#This Row],[ID]]&amp;""", ""functor"" : """ &amp;Table6[[#This Row],[L1]]&amp;""",  ""components"" : [",IF(Table6[[#This Row],[Type]]="]},","]}, ",IF(Table6[[#This Row],[Type]]="]}","]}",IF(MATCH(Table6[[#This Row],[Type]],{"integer","float","string","date","boolean"},0),"{""id"" : """&amp;Table6[[#This Row],[ID]]&amp;""" , ""functor"" : """&amp;Table6[[#This Row],[L1]]&amp;""" , ""components"": [ { ""value"": """ &amp; Table6[[#This Row],[Value]]&amp;""", ""type"" : """&amp;Table6[[#This Row],[Type]]&amp;""" } ] } "&amp;IF(OR($C3="]}",$C3="]},"),""," , ")))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -30369,13 +30379,13 @@
         <v>2001</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>2443</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>2447</v>
+        <v>2445</v>
       </c>
       <c r="E2" s="96" t="s">
         <v>2272</v>
@@ -30426,13 +30436,13 @@
         <v>1999</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>2448</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>2446</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>2444</v>
-      </c>
       <c r="D3" s="5" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="E3" s="96" t="s">
         <v>2272</v>
@@ -30475,7 +30485,64 @@
       </c>
       <c r="R3" s="5" t="str">
         <f>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": """&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skills]]&amp;""": "&amp;Table5[[#This Row],[skills]]&amp;", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referents]]&amp;""": "&amp;Table5[[#This Row],[referents]]&amp;", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</f>
-        <v>{"id": "e231791e-2719-4503-ad8f-8dd55a53901e", "type": "Part-Time", "summary": "Developers for a Framework for developing p2p Front-Ends for Blockchain APPs", "description": "We invite you to join Fermat, a community building an OS extension able to run p2p mobile APPs  like Uber without Uber Inc., or  Airbnb without Airbnb Inc , or Linkedin, or Tinder, etc,  you name it, all of them without the middle-men.  Each component of the system is owned by whoever writes their code. Later, devs receive a stream of micro-payments from end-users around the globe using APPs built with their components.  Join us and learn bitcoin and blockchain technology and be part of one of the fastest growing open source projects.: https://github.com/Fermat-ORG/fermat ...", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skills": [{"skillId": "4416192b-9dec-49b0-9d13-fb0815af6c3f", "skillName":"Java"}, {"skillId": "3c91c578-2d39-42d4-adb0-9071d9eb116a", "skillName":"Financial Apps"}, {"skillId": "b48bfe5a-15fa-4d8e-b253-752b51c2b94b", "skillName":"cryptography"}], "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referents": [{"referentId":"40c96981-ca91-4083-9dfc-76826df0f432", "referentName":"Britta"},{"referentId":"c6a3c02e-5724-4a35-adc7-ddc37d3c721b","referentName":"Jane Best"}], "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
+        <v>{"id": "e231791e-2719-4503-ad8f-8dd55a53901e", "type": "Contest", "summary": "Contest – online sales team/tools for bitcoin development", "description": "To join this contest just register at https://www.greatcoincontest.io, click at the product you want to sell and generate your reff link. This reff link also works with other products on the site. Once your id is in buyer’s cookies, you’ll get 10% of every sale from this person on the marketplace.  When? Contest starts 24.2. 2016 0:00 UTC and ends 24.3. 2016 23:59 UTC. Winner will be contacted right after that. ...", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skills": [{"skillId": "4416192b-9dec-49b0-9d13-fb0815af6c3f", "skillName":"Java"}, {"skillId": "3c91c578-2d39-42d4-adb0-9071d9eb116a", "skillName":"Financial Apps"}, {"skillId": "b48bfe5a-15fa-4d8e-b253-752b51c2b94b", "skillName":"cryptography"}], "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referents": [{"referentId":"40c96981-ca91-4083-9dfc-76826df0f432", "referentName":"Britta"},{"referentId":"c6a3c02e-5724-4a35-adc7-ddc37d3c721b","referentName":"Jane Best"}], "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2450</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2444</v>
+      </c>
+      <c r="C4" s="118" t="s">
+        <v>2449</v>
+      </c>
+      <c r="D4" s="118" t="s">
+        <v>2451</v>
+      </c>
+      <c r="E4" s="96" t="s">
+        <v>2272</v>
+      </c>
+      <c r="F4" s="96" t="s">
+        <v>2272</v>
+      </c>
+      <c r="G4" s="96" t="s">
+        <v>2272</v>
+      </c>
+      <c r="H4" s="96" t="s">
+        <v>2272</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>2070</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>2362</v>
+      </c>
+      <c r="K4" s="67" t="s">
+        <v>2310</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>2436</v>
+      </c>
+      <c r="M4" s="67" t="s">
+        <v>2271</v>
+      </c>
+      <c r="N4" s="67" t="s">
+        <v>2366</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>2441</v>
+      </c>
+      <c r="P4" s="67" t="s">
+        <v>2000</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>2350.3000000000002</v>
+      </c>
+      <c r="R4" s="5" t="str">
+        <f>"{"""&amp;Table5[[#Headers],[id]]&amp;""": """&amp;Table5[[#This Row],[id]]&amp;""", """&amp;Table5[[#Headers],[type]]&amp;""": """&amp;Table5[[#This Row],[type]]&amp;""", """&amp;Table5[[#Headers],[summary]]&amp;""": """&amp;Table5[[#This Row],[summary]]&amp;""", """&amp;Table5[[#Headers],[description]]&amp;""": """&amp;Table5[[#This Row],[description]]&amp;""", """&amp;Table5[[#Headers],[postedDate]]&amp;""": """&amp;Table5[[#This Row],[postedDate]]&amp;""", """&amp;Table5[[#Headers],[broadcastDate]]&amp;""": """&amp;Table5[[#This Row],[broadcastDate]]&amp;""", """&amp;Table5[[#Headers],[startDate]]&amp;""": """&amp;Table5[[#This Row],[startDate]]&amp;""", """&amp;Table5[[#Headers],[endDate]]&amp;""": """&amp;Table5[[#This Row],[endDate]]&amp;""", """&amp;Table5[[#Headers],[currency]]&amp;""": """&amp;Table5[[#This Row],[currency]]&amp;""", """&amp;Table5[[#Headers],[location]]&amp;""": """&amp;Table5[[#This Row],[location]]&amp;""", """&amp;Table5[[#Headers],[isPayoutInPieces]]&amp;""": """&amp;Table5[[#This Row],[isPayoutInPieces]]&amp;""", """&amp;Table5[[#Headers],[skills]]&amp;""": "&amp;Table5[[#This Row],[skills]]&amp;", """&amp;Table5[[#Headers],[posterId]]&amp;""": """&amp;Table5[[#This Row],[posterId]]&amp;""", """&amp;Table5[[#Headers],[canForward]]&amp;""": """&amp;Table5[[#This Row],[canForward]]&amp;""", """&amp;Table5[[#Headers],[referents]]&amp;""": "&amp;Table5[[#This Row],[referents]]&amp;", """&amp;Table5[[#Headers],[contractType]]&amp;""": """&amp;Table5[[#This Row],[contractType]]&amp;""", """&amp;Table5[[#Headers],[budget]]&amp;""": """&amp;Table5[[#This Row],[budget]]&amp;"""},"</f>
+        <v>{"id": "e231791e-2719-4503-ad8f-8dd55a53901a", "type": "Project-Hourly", "summary": "Help test Bitcoin as payment for my travel-related business", "description": "This project can be a huge project but same time can easily fail, so please PM with your skills, I will provide you the project details and if you consider it’s a good idea we can start work right away", "postedDate": "2002-05-30T09:30:10Z", "broadcastDate": "2002-05-30T09:30:10Z", "startDate": "2002-05-30T09:30:10Z", "endDate": "2002-05-30T09:30:10Z", "currency": "USD", "location": "United States", "isPayoutInPieces": "false", "skills": [{"skillId": "4416192b-9dec-49b0-9d13-fb0815af6c3f", "skillName":"Java"}, {"skillId": "3c91c578-2d39-42d4-adb0-9071d9eb116a", "skillName":"Financial Apps"}, {"skillId": "b48bfe5a-15fa-4d8e-b253-752b51c2b94b", "skillName":"cryptography"}], "posterId": "eeeeeeee-eeee-eeee-eeee-eeeeeeeeeeee", "canForward": "true", "referents": [{"referentId":"40c96981-ca91-4083-9dfc-76826df0f432", "referentName":"Britta"},{"referentId":"c6a3c02e-5724-4a35-adc7-ddc37d3c721b","referentName":"Jane Best"}], "contractType": "23940120-4943-4462-9c46-2b23ef94108c", "budget": "2350.3"},</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -30528,8 +30595,9 @@
     <hyperlink ref="B16" r:id="rId1" location="ad-output"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>